<commit_message>
add affiliated client tab and functionality, update styles for active and success states
</commit_message>
<xml_diff>
--- a/קבצי אקסל/לקוחות מצורפים.xlsx
+++ b/קבצי אקסל/לקוחות מצורפים.xlsx
@@ -448,10 +448,10 @@
         <v>258147369</v>
       </c>
       <c r="G2" t="str">
-        <v>חכם</v>
+        <v>רגיל</v>
       </c>
       <c r="H2" t="str">
-        <v>1975-05-03</v>
+        <v>1975-05-21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>